<commit_message>
project report fix est act
</commit_message>
<xml_diff>
--- a/Base/src/main/resources/templates/projectDetailsBySkills.xlsx
+++ b/Base/src/main/resources/templates/projectDetailsBySkills.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20373"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20375"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\FS-Workspace\bops\Base\src\main\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8359580-EDD3-43C6-A4D3-3D3A9370D640}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF68AF44-9875-4C80-A684-8D1C07DF3925}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16650" windowHeight="4950" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="66">
   <si>
     <t>Client Name</t>
   </si>
@@ -212,9 +212,6 @@
     <t>Client Partner</t>
   </si>
   <si>
-    <t xml:space="preserve">Internal team </t>
-  </si>
-  <si>
     <t>Estimated Revenue</t>
   </si>
   <si>
@@ -230,7 +227,10 @@
     <t>Revenue</t>
   </si>
   <si>
-    <t>Project Type</t>
+    <t xml:space="preserve">Project Type </t>
+  </si>
+  <si>
+    <t>Project Sub Type</t>
   </si>
 </sst>
 </file>
@@ -396,17 +396,17 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -953,13 +953,13 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="CY7" sqref="CY7"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="16.26171875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.41796875" style="21" customWidth="1"/>
+    <col min="2" max="2" width="13.5234375" style="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.68359375" style="5" customWidth="1"/>
     <col min="4" max="4" width="16.15625" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.41796875" style="5" bestFit="1" customWidth="1"/>
@@ -1085,122 +1085,122 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:210" x14ac:dyDescent="0.55000000000000004">
-      <c r="N1" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19" t="s">
+      <c r="N1" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="19"/>
-      <c r="W1" s="19"/>
-      <c r="X1" s="19"/>
-      <c r="Y1" s="19"/>
-      <c r="Z1" s="19"/>
-      <c r="AA1" s="19"/>
-      <c r="AB1" s="19"/>
-      <c r="AC1" s="19"/>
-      <c r="AD1" s="19" t="s">
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="21"/>
+      <c r="T1" s="21"/>
+      <c r="U1" s="21"/>
+      <c r="V1" s="21"/>
+      <c r="W1" s="21"/>
+      <c r="X1" s="21"/>
+      <c r="Y1" s="21"/>
+      <c r="Z1" s="21"/>
+      <c r="AA1" s="21"/>
+      <c r="AB1" s="21"/>
+      <c r="AC1" s="21"/>
+      <c r="AD1" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="AE1" s="19"/>
-      <c r="AF1" s="19"/>
-      <c r="AG1" s="19"/>
-      <c r="AH1" s="19"/>
-      <c r="AI1" s="19"/>
-      <c r="AJ1" s="19"/>
-      <c r="AK1" s="19"/>
-      <c r="AL1" s="19"/>
-      <c r="AM1" s="19"/>
-      <c r="AN1" s="19"/>
-      <c r="AO1" s="19"/>
-      <c r="AP1" s="19"/>
-      <c r="AQ1" s="19"/>
-      <c r="AR1" s="19" t="s">
+      <c r="AE1" s="21"/>
+      <c r="AF1" s="21"/>
+      <c r="AG1" s="21"/>
+      <c r="AH1" s="21"/>
+      <c r="AI1" s="21"/>
+      <c r="AJ1" s="21"/>
+      <c r="AK1" s="21"/>
+      <c r="AL1" s="21"/>
+      <c r="AM1" s="21"/>
+      <c r="AN1" s="21"/>
+      <c r="AO1" s="21"/>
+      <c r="AP1" s="21"/>
+      <c r="AQ1" s="21"/>
+      <c r="AR1" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS1" s="21"/>
+      <c r="AT1" s="21"/>
+      <c r="AU1" s="21"/>
+      <c r="AV1" s="21"/>
+      <c r="AW1" s="21"/>
+      <c r="AX1" s="21"/>
+      <c r="AY1" s="21"/>
+      <c r="AZ1" s="21"/>
+      <c r="BA1" s="21"/>
+      <c r="BB1" s="21"/>
+      <c r="BC1" s="21"/>
+      <c r="BD1" s="21"/>
+      <c r="BE1" s="21"/>
+      <c r="BG1" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="BH1" s="21"/>
+      <c r="BI1" s="21"/>
+      <c r="BJ1" s="21"/>
+      <c r="BK1" s="21"/>
+      <c r="BL1" s="21"/>
+      <c r="BM1" s="21"/>
+      <c r="BN1" s="21"/>
+      <c r="BO1" s="21"/>
+      <c r="BP1" s="21"/>
+      <c r="BQ1" s="21"/>
+      <c r="BR1" s="21"/>
+      <c r="BS1" s="21"/>
+      <c r="BT1" s="21"/>
+      <c r="BU1" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="BV1" s="21"/>
+      <c r="BW1" s="21"/>
+      <c r="BX1" s="21"/>
+      <c r="BY1" s="21"/>
+      <c r="BZ1" s="21"/>
+      <c r="CA1" s="21"/>
+      <c r="CB1" s="21"/>
+      <c r="CC1" s="21"/>
+      <c r="CD1" s="21"/>
+      <c r="CE1" s="21"/>
+      <c r="CF1" s="21"/>
+      <c r="CG1" s="21"/>
+      <c r="CH1" s="21"/>
+      <c r="CI1" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="AS1" s="19"/>
-      <c r="AT1" s="19"/>
-      <c r="AU1" s="19"/>
-      <c r="AV1" s="19"/>
-      <c r="AW1" s="19"/>
-      <c r="AX1" s="19"/>
-      <c r="AY1" s="19"/>
-      <c r="AZ1" s="19"/>
-      <c r="BA1" s="19"/>
-      <c r="BB1" s="19"/>
-      <c r="BC1" s="19"/>
-      <c r="BD1" s="19"/>
-      <c r="BE1" s="19"/>
-      <c r="BG1" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="BH1" s="19"/>
-      <c r="BI1" s="19"/>
-      <c r="BJ1" s="19"/>
-      <c r="BK1" s="19"/>
-      <c r="BL1" s="19"/>
-      <c r="BM1" s="19"/>
-      <c r="BN1" s="19"/>
-      <c r="BO1" s="19"/>
-      <c r="BP1" s="19"/>
-      <c r="BQ1" s="19"/>
-      <c r="BR1" s="19"/>
-      <c r="BS1" s="19"/>
-      <c r="BT1" s="19"/>
-      <c r="BU1" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="BV1" s="19"/>
-      <c r="BW1" s="19"/>
-      <c r="BX1" s="19"/>
-      <c r="BY1" s="19"/>
-      <c r="BZ1" s="19"/>
-      <c r="CA1" s="19"/>
-      <c r="CB1" s="19"/>
-      <c r="CC1" s="19"/>
-      <c r="CD1" s="19"/>
-      <c r="CE1" s="19"/>
-      <c r="CF1" s="19"/>
-      <c r="CG1" s="19"/>
-      <c r="CH1" s="19"/>
-      <c r="CI1" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="CJ1" s="20"/>
-      <c r="CK1" s="20"/>
-      <c r="CL1" s="20"/>
-      <c r="CM1" s="20"/>
-      <c r="CN1" s="20"/>
-      <c r="CO1" s="20"/>
-      <c r="CP1" s="20"/>
-      <c r="CQ1" s="20"/>
-      <c r="CR1" s="20"/>
-      <c r="CS1" s="20"/>
-      <c r="CT1" s="20"/>
-      <c r="CU1" s="20"/>
-      <c r="CV1" s="20"/>
+      <c r="CJ1" s="22"/>
+      <c r="CK1" s="22"/>
+      <c r="CL1" s="22"/>
+      <c r="CM1" s="22"/>
+      <c r="CN1" s="22"/>
+      <c r="CO1" s="22"/>
+      <c r="CP1" s="22"/>
+      <c r="CQ1" s="22"/>
+      <c r="CR1" s="22"/>
+      <c r="CS1" s="22"/>
+      <c r="CT1" s="22"/>
+      <c r="CU1" s="22"/>
+      <c r="CV1" s="22"/>
       <c r="CX1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="DC1" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="DD1" s="19"/>
-      <c r="DE1" s="19"/>
-      <c r="DF1" s="19"/>
-      <c r="DG1" s="19"/>
+      <c r="DC1" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="DD1" s="21"/>
+      <c r="DE1" s="21"/>
+      <c r="DF1" s="21"/>
+      <c r="DG1" s="21"/>
     </row>
     <row r="2" spans="1:210" s="7" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B2" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="20" t="s">
         <v>65</v>
       </c>
       <c r="C2" s="8" t="s">
@@ -1240,7 +1240,7 @@
         <v>21</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P2" s="10" t="s">
         <v>32</v>
@@ -1498,7 +1498,7 @@
         <v>56</v>
       </c>
       <c r="CW2" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="CX2" s="15" t="s">
         <v>30</v>

</xml_diff>